<commit_message>
Added logic to set TSW eersion and platform
</commit_message>
<xml_diff>
--- a/ToolkitForTSW/SQL/AnnotatedSettingsList.xlsx
+++ b/ToolkitForTSW/SQL/AnnotatedSettingsList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\ToolkitForTSW\ToolkitForTSW\SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/60d6ce76cb6667a7/Projecten/ToolkitForTSW/ToolkitForTSW/SQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E2B20-B2CC-48B7-8BF6-73167ACC8DAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{601E2B20-B2CC-48B7-8BF6-73167ACC8DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F4D9702-FBF6-4BDF-BFE1-BFC6238E73DC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{191BE9AA-23A1-4541-84A4-20F2DD8F8049}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="28800" windowHeight="15435" xr2:uid="{191BE9AA-23A1-4541-84A4-20F2DD8F8049}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="1278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1494" uniqueCount="1279">
   <si>
     <t>a.ParallelAnimEvaluation</t>
   </si>
@@ -3859,6 +3859,9 @@
   </si>
   <si>
     <t>The number of blocks to compress in parallel for DXT compression.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -4228,8 +4231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16165DDD-041B-4041-9F77-C773BC8EEED6}">
   <dimension ref="A1:B954"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A940" workbookViewId="0">
+      <selection activeCell="B205" sqref="B205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4696,13 +4699,17 @@
       <c r="A64" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
@@ -5506,7 +5513,9 @@
       <c r="A175" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B175" s="1"/>
+      <c r="B175" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="2" t="s">
@@ -5706,7 +5715,9 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="3"/>
-      <c r="B205" s="1"/>
+      <c r="B205" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="3"/>
@@ -5716,7 +5727,9 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="3"/>
-      <c r="B207" s="1"/>
+      <c r="B207" s="1" t="s">
+        <v>1278</v>
+      </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="3"/>
@@ -11034,162 +11047,6 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A15:A23"/>
-    <mergeCell ref="A28:A35"/>
-    <mergeCell ref="A48:A51"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A105:A106"/>
-    <mergeCell ref="A107:A109"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="A118:A120"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="A181:A184"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="A188:A194"/>
-    <mergeCell ref="A195:A197"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A143:A144"/>
-    <mergeCell ref="A145:A148"/>
-    <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A155:A156"/>
-    <mergeCell ref="A165:A167"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="A255:A257"/>
-    <mergeCell ref="A259:A260"/>
-    <mergeCell ref="A265:A268"/>
-    <mergeCell ref="A269:A272"/>
-    <mergeCell ref="A273:A274"/>
-    <mergeCell ref="A275:A276"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A204:A226"/>
-    <mergeCell ref="A227:A246"/>
-    <mergeCell ref="A247:A248"/>
-    <mergeCell ref="A249:A251"/>
-    <mergeCell ref="A252:A253"/>
-    <mergeCell ref="A303:A306"/>
-    <mergeCell ref="A307:A309"/>
-    <mergeCell ref="A310:A312"/>
-    <mergeCell ref="A313:A316"/>
-    <mergeCell ref="A317:A319"/>
-    <mergeCell ref="A320:A322"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="A281:A287"/>
-    <mergeCell ref="A289:A291"/>
-    <mergeCell ref="A292:A297"/>
-    <mergeCell ref="A298:A302"/>
-    <mergeCell ref="A350:A351"/>
-    <mergeCell ref="A353:A356"/>
-    <mergeCell ref="A357:A358"/>
-    <mergeCell ref="A359:A361"/>
-    <mergeCell ref="A362:A367"/>
-    <mergeCell ref="A368:A369"/>
-    <mergeCell ref="A323:A325"/>
-    <mergeCell ref="A326:A328"/>
-    <mergeCell ref="A331:A332"/>
-    <mergeCell ref="A333:A336"/>
-    <mergeCell ref="A337:A340"/>
-    <mergeCell ref="A343:A344"/>
-    <mergeCell ref="A407:A409"/>
-    <mergeCell ref="A410:A411"/>
-    <mergeCell ref="A413:A416"/>
-    <mergeCell ref="A417:A419"/>
-    <mergeCell ref="A420:A423"/>
-    <mergeCell ref="A425:A429"/>
-    <mergeCell ref="A376:A378"/>
-    <mergeCell ref="A380:A383"/>
-    <mergeCell ref="A384:A385"/>
-    <mergeCell ref="A389:A393"/>
-    <mergeCell ref="A394:A399"/>
-    <mergeCell ref="A402:A406"/>
-    <mergeCell ref="A453:A456"/>
-    <mergeCell ref="A457:A461"/>
-    <mergeCell ref="A462:A464"/>
-    <mergeCell ref="A469:A471"/>
-    <mergeCell ref="A473:A476"/>
-    <mergeCell ref="A490:A491"/>
-    <mergeCell ref="A430:A433"/>
-    <mergeCell ref="A434:A435"/>
-    <mergeCell ref="A436:A438"/>
-    <mergeCell ref="A439:A444"/>
-    <mergeCell ref="A445:A446"/>
-    <mergeCell ref="A448:A450"/>
-    <mergeCell ref="A507:A511"/>
-    <mergeCell ref="A512:A516"/>
-    <mergeCell ref="A518:A519"/>
-    <mergeCell ref="A522:A525"/>
-    <mergeCell ref="A531:A532"/>
-    <mergeCell ref="A535:A538"/>
-    <mergeCell ref="A492:A493"/>
-    <mergeCell ref="A494:A497"/>
-    <mergeCell ref="A498:A499"/>
-    <mergeCell ref="A500:A501"/>
-    <mergeCell ref="A502:A504"/>
-    <mergeCell ref="A505:A506"/>
-    <mergeCell ref="A561:A565"/>
-    <mergeCell ref="A568:A570"/>
-    <mergeCell ref="A571:A574"/>
-    <mergeCell ref="A575:A577"/>
-    <mergeCell ref="A579:A580"/>
-    <mergeCell ref="A581:A582"/>
-    <mergeCell ref="A539:A542"/>
-    <mergeCell ref="A543:A547"/>
-    <mergeCell ref="A550:A552"/>
-    <mergeCell ref="A553:A555"/>
-    <mergeCell ref="A556:A558"/>
-    <mergeCell ref="A559:A560"/>
-    <mergeCell ref="A611:A613"/>
-    <mergeCell ref="A614:A617"/>
-    <mergeCell ref="A618:A622"/>
-    <mergeCell ref="A629:A632"/>
-    <mergeCell ref="A636:A637"/>
-    <mergeCell ref="A638:A641"/>
-    <mergeCell ref="A587:A588"/>
-    <mergeCell ref="A591:A598"/>
-    <mergeCell ref="A599:A600"/>
-    <mergeCell ref="A601:A602"/>
-    <mergeCell ref="A603:A607"/>
-    <mergeCell ref="A608:A610"/>
-    <mergeCell ref="A679:A682"/>
-    <mergeCell ref="A683:A687"/>
-    <mergeCell ref="A688:A695"/>
-    <mergeCell ref="A696:A697"/>
-    <mergeCell ref="A698:A699"/>
-    <mergeCell ref="A700:A702"/>
-    <mergeCell ref="A645:A647"/>
-    <mergeCell ref="A651:A653"/>
-    <mergeCell ref="A659:A660"/>
-    <mergeCell ref="A661:A662"/>
-    <mergeCell ref="A670:A671"/>
-    <mergeCell ref="A674:A676"/>
-    <mergeCell ref="A731:A732"/>
-    <mergeCell ref="A736:A737"/>
-    <mergeCell ref="A738:A739"/>
-    <mergeCell ref="A742:A744"/>
-    <mergeCell ref="A745:A747"/>
-    <mergeCell ref="A748:A752"/>
-    <mergeCell ref="A703:A708"/>
-    <mergeCell ref="A710:A712"/>
-    <mergeCell ref="A713:A716"/>
-    <mergeCell ref="A719:A721"/>
-    <mergeCell ref="A725:A727"/>
-    <mergeCell ref="A729:A730"/>
     <mergeCell ref="A804:A805"/>
     <mergeCell ref="A951:A952"/>
     <mergeCell ref="A792:A793"/>
@@ -11204,6 +11061,162 @@
     <mergeCell ref="A764:A766"/>
     <mergeCell ref="A770:A772"/>
     <mergeCell ref="A773:A774"/>
+    <mergeCell ref="A731:A732"/>
+    <mergeCell ref="A736:A737"/>
+    <mergeCell ref="A738:A739"/>
+    <mergeCell ref="A742:A744"/>
+    <mergeCell ref="A745:A747"/>
+    <mergeCell ref="A748:A752"/>
+    <mergeCell ref="A703:A708"/>
+    <mergeCell ref="A710:A712"/>
+    <mergeCell ref="A713:A716"/>
+    <mergeCell ref="A719:A721"/>
+    <mergeCell ref="A725:A727"/>
+    <mergeCell ref="A729:A730"/>
+    <mergeCell ref="A679:A682"/>
+    <mergeCell ref="A683:A687"/>
+    <mergeCell ref="A688:A695"/>
+    <mergeCell ref="A696:A697"/>
+    <mergeCell ref="A698:A699"/>
+    <mergeCell ref="A700:A702"/>
+    <mergeCell ref="A645:A647"/>
+    <mergeCell ref="A651:A653"/>
+    <mergeCell ref="A659:A660"/>
+    <mergeCell ref="A661:A662"/>
+    <mergeCell ref="A670:A671"/>
+    <mergeCell ref="A674:A676"/>
+    <mergeCell ref="A611:A613"/>
+    <mergeCell ref="A614:A617"/>
+    <mergeCell ref="A618:A622"/>
+    <mergeCell ref="A629:A632"/>
+    <mergeCell ref="A636:A637"/>
+    <mergeCell ref="A638:A641"/>
+    <mergeCell ref="A587:A588"/>
+    <mergeCell ref="A591:A598"/>
+    <mergeCell ref="A599:A600"/>
+    <mergeCell ref="A601:A602"/>
+    <mergeCell ref="A603:A607"/>
+    <mergeCell ref="A608:A610"/>
+    <mergeCell ref="A561:A565"/>
+    <mergeCell ref="A568:A570"/>
+    <mergeCell ref="A571:A574"/>
+    <mergeCell ref="A575:A577"/>
+    <mergeCell ref="A579:A580"/>
+    <mergeCell ref="A581:A582"/>
+    <mergeCell ref="A539:A542"/>
+    <mergeCell ref="A543:A547"/>
+    <mergeCell ref="A550:A552"/>
+    <mergeCell ref="A553:A555"/>
+    <mergeCell ref="A556:A558"/>
+    <mergeCell ref="A559:A560"/>
+    <mergeCell ref="A507:A511"/>
+    <mergeCell ref="A512:A516"/>
+    <mergeCell ref="A518:A519"/>
+    <mergeCell ref="A522:A525"/>
+    <mergeCell ref="A531:A532"/>
+    <mergeCell ref="A535:A538"/>
+    <mergeCell ref="A492:A493"/>
+    <mergeCell ref="A494:A497"/>
+    <mergeCell ref="A498:A499"/>
+    <mergeCell ref="A500:A501"/>
+    <mergeCell ref="A502:A504"/>
+    <mergeCell ref="A505:A506"/>
+    <mergeCell ref="A453:A456"/>
+    <mergeCell ref="A457:A461"/>
+    <mergeCell ref="A462:A464"/>
+    <mergeCell ref="A469:A471"/>
+    <mergeCell ref="A473:A476"/>
+    <mergeCell ref="A490:A491"/>
+    <mergeCell ref="A430:A433"/>
+    <mergeCell ref="A434:A435"/>
+    <mergeCell ref="A436:A438"/>
+    <mergeCell ref="A439:A444"/>
+    <mergeCell ref="A445:A446"/>
+    <mergeCell ref="A448:A450"/>
+    <mergeCell ref="A407:A409"/>
+    <mergeCell ref="A410:A411"/>
+    <mergeCell ref="A413:A416"/>
+    <mergeCell ref="A417:A419"/>
+    <mergeCell ref="A420:A423"/>
+    <mergeCell ref="A425:A429"/>
+    <mergeCell ref="A376:A378"/>
+    <mergeCell ref="A380:A383"/>
+    <mergeCell ref="A384:A385"/>
+    <mergeCell ref="A389:A393"/>
+    <mergeCell ref="A394:A399"/>
+    <mergeCell ref="A402:A406"/>
+    <mergeCell ref="A350:A351"/>
+    <mergeCell ref="A353:A356"/>
+    <mergeCell ref="A357:A358"/>
+    <mergeCell ref="A359:A361"/>
+    <mergeCell ref="A362:A367"/>
+    <mergeCell ref="A368:A369"/>
+    <mergeCell ref="A323:A325"/>
+    <mergeCell ref="A326:A328"/>
+    <mergeCell ref="A331:A332"/>
+    <mergeCell ref="A333:A336"/>
+    <mergeCell ref="A337:A340"/>
+    <mergeCell ref="A343:A344"/>
+    <mergeCell ref="A303:A306"/>
+    <mergeCell ref="A307:A309"/>
+    <mergeCell ref="A310:A312"/>
+    <mergeCell ref="A313:A316"/>
+    <mergeCell ref="A317:A319"/>
+    <mergeCell ref="A320:A322"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="A281:A287"/>
+    <mergeCell ref="A289:A291"/>
+    <mergeCell ref="A292:A297"/>
+    <mergeCell ref="A298:A302"/>
+    <mergeCell ref="A255:A257"/>
+    <mergeCell ref="A259:A260"/>
+    <mergeCell ref="A265:A268"/>
+    <mergeCell ref="A269:A272"/>
+    <mergeCell ref="A273:A274"/>
+    <mergeCell ref="A275:A276"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A204:A226"/>
+    <mergeCell ref="A227:A246"/>
+    <mergeCell ref="A247:A248"/>
+    <mergeCell ref="A249:A251"/>
+    <mergeCell ref="A252:A253"/>
+    <mergeCell ref="A178:A179"/>
+    <mergeCell ref="A181:A184"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="A188:A194"/>
+    <mergeCell ref="A195:A197"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A143:A144"/>
+    <mergeCell ref="A145:A148"/>
+    <mergeCell ref="A149:A152"/>
+    <mergeCell ref="A155:A156"/>
+    <mergeCell ref="A165:A167"/>
+    <mergeCell ref="A168:A169"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A105:A106"/>
+    <mergeCell ref="A107:A109"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="A118:A120"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A23"/>
+    <mergeCell ref="A28:A35"/>
+    <mergeCell ref="A48:A51"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="A59:A61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>